<commit_message>
Cambios del sprint 1
</commit_message>
<xml_diff>
--- a/docs/sprint 1/Sprint 1 Backlog -  Sprint 1 Planning.xlsx
+++ b/docs/sprint 1/Sprint 1 Backlog -  Sprint 1 Planning.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\La_U\Ing SW II\Proyecto Final\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caro\Documents\NetBeansProjects\xtremescrump\docs\sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Backlog V1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Dia 4</t>
   </si>
@@ -87,12 +87,6 @@
     <t xml:space="preserve">Actualizar el product backlog, mostrando nombre y prioridad de la historia de usuario. </t>
   </si>
   <si>
-    <t>Se prensentará una panatalla para la creación del proyecto, nombre y fecha de incio</t>
-  </si>
-  <si>
-    <t>Se prensentará una panatalla para agregar los mails de los miembros del equipo</t>
-  </si>
-  <si>
     <t>XÑ - CL</t>
   </si>
   <si>
@@ -166,6 +160,57 @@
   </si>
   <si>
     <t>Se presentara un Error sino se ingresa todos los datos</t>
+  </si>
+  <si>
+    <t>Yo como scrum master deseo crear el proyecto Xtreme Scrum</t>
+  </si>
+  <si>
+    <t>Crear la pantalla de proyecto</t>
+  </si>
+  <si>
+    <t>Crear una tabla que muestre los proyectos</t>
+  </si>
+  <si>
+    <t>-Se prensentará una pantalla para la administración de proyectos.
+-Aparecerá un botón 'Nuevo Proyecto', que permitirá crear nuevos proyectos.</t>
+  </si>
+  <si>
+    <t>- Se presentará una tabla con los proyectos creados - nombre, descripción, fecha inicio, fecha fin
+- Si no existen proyectos creados, se presentará un mensaje en la tabla que diga: 'No existen registros'
+- Cada registro tendrá botones de edición y eliminación, en la última columna de la tabla llamada 'Opciones'</t>
+  </si>
+  <si>
+    <t>Desplegar un diálogo  para la creación de nuevos proyectos</t>
+  </si>
+  <si>
+    <t>- Al hacer clic en el botón 'Nuevo Proyecto' se desplegará un diálogo con el formato de historia de usuario.
+- En el diálogo se mostrará campos de: Nombre, Descripción, Fecha Inicio, Fecha Fin.
+- El diálogo tendrá botones de guadar y cancelar.</t>
+  </si>
+  <si>
+    <t>Guardar proyecto</t>
+  </si>
+  <si>
+    <t>- Todos los campos requeridos deben ser ingresados para poder guardar el proyecto.
+- Los campos requeridos, aparecerán con * de color rojo.
+- Si se intenta guardar el proyecto, aparecerán mensajes de error en la esquina superior derecha de la pantalla, mostrando el campo requerido que no ha sido ingresado.
+- Al guardar el proyecto, se refrescará la tabla mostrando el proyecto ingresado.</t>
+  </si>
+  <si>
+    <t>Editar proyecto existente</t>
+  </si>
+  <si>
+    <t>- Al hacer clic en el botón editar, que es un botón con el signo de un lápiz, aparece un diálogo con el mismo formato de nuevo proyecto, pero con los campos llenos del proyeco seleccionado.
+- Al tratar de guardar los cambios de la edición, se validará que los campos requeridos esten llenos. Mostrando mensajes de error de los campos requeridos no ingresados.
+- Si se cancela la edición, los datos quedarán en la tabla como antes de la edición.
+- Cuando se guarde la edición, se refrescará la tabla mostrando en el proyecto seleccionado, los nuevos datos.</t>
+  </si>
+  <si>
+    <t>Eliminar proyecto existente</t>
+  </si>
+  <si>
+    <t>- Al hacer clic en el botón eliminar, que es un botón con el signo de un tacho de basura, aparece un diálogo que pregunta la confirmación de la eliminación. Esta confirmación tiene los botones SI y NO.
+- Al hacer clic en SI, aparece un mensaje de 'Error en la eliminación del proyecto ' si dicho proyecto tiene historias de usuario ligadas.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +480,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -472,73 +517,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,12 +532,95 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -562,40 +630,35 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -918,11 +981,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1122132528"/>
-        <c:axId val="-1122128720"/>
+        <c:axId val="230558432"/>
+        <c:axId val="230553728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1122132528"/>
+        <c:axId val="230558432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,12 +1098,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1122128720"/>
+        <c:crossAx val="230553728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1122128720"/>
+        <c:axId val="230553728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,7 +1216,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1122132528"/>
+        <c:crossAx val="230558432"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2056,9 +2119,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:F9"/>
     </sheetView>
   </sheetViews>
@@ -2071,11 +2134,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="B1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -2085,7 +2148,7 @@
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>7</v>
@@ -2093,119 +2156,171 @@
       <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+    <row r="5" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
     </row>
-    <row r="6" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
+    <row r="6" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46"/>
     </row>
-    <row r="7" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+    </row>
+    <row r="8" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+    </row>
+    <row r="9" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="63"/>
+      <c r="F9" s="64"/>
+    </row>
+    <row r="10" spans="1:10" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
+    </row>
+    <row r="11" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="31" t="s">
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
-    <row r="8" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="34" t="s">
+    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D9:F9"/>
+  <mergeCells count="18">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2240,19 +2355,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="B1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="B1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
     </row>
     <row r="2" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2293,10 +2408,10 @@
     </row>
     <row r="4" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2310,448 +2425,448 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
     </row>
     <row r="7" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="40" t="s">
+      <c r="E7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="41" t="s">
+      <c r="G7" s="51"/>
+      <c r="H7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="41" t="s">
+      <c r="L7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="M7" s="41" t="s">
+      <c r="M7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="P7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="Q7" s="20" t="s">
         <v>28</v>
-      </c>
-      <c r="P7" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="41" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="47" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="43">
+      <c r="D8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="52">
         <v>4</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="54">
+      <c r="G8" s="52"/>
+      <c r="H8" s="24">
         <v>4</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="17">
         <v>4</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="17">
         <v>4</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="17">
         <v>4</v>
       </c>
-      <c r="L8" s="37">
+      <c r="L8" s="17">
         <v>0</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="17">
         <v>0</v>
       </c>
-      <c r="N8" s="37">
+      <c r="N8" s="17">
         <v>0</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="17">
         <v>0</v>
       </c>
-      <c r="P8" s="37">
+      <c r="P8" s="17">
         <v>0</v>
       </c>
-      <c r="Q8" s="37">
+      <c r="Q8" s="17">
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43">
+      <c r="D9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="52">
         <v>8</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="54">
+      <c r="G9" s="52"/>
+      <c r="H9" s="24">
         <v>8</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="17">
         <v>8</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="17">
         <v>4</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="17">
         <v>4</v>
       </c>
-      <c r="L9" s="37">
+      <c r="L9" s="17">
         <v>4</v>
       </c>
-      <c r="M9" s="37">
+      <c r="M9" s="17">
         <v>4</v>
       </c>
-      <c r="N9" s="37">
+      <c r="N9" s="17">
         <v>4</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="17">
         <v>4</v>
       </c>
-      <c r="P9" s="37">
+      <c r="P9" s="17">
         <v>4</v>
       </c>
-      <c r="Q9" s="37">
+      <c r="Q9" s="17">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="44">
+      <c r="D10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="53">
         <v>7</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="55">
+      <c r="G10" s="54"/>
+      <c r="H10" s="25">
         <v>7</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="17">
         <v>7</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="17">
         <v>7</v>
       </c>
-      <c r="K10" s="37">
+      <c r="K10" s="17">
         <v>7</v>
       </c>
-      <c r="L10" s="46">
+      <c r="L10" s="22">
         <v>7</v>
       </c>
-      <c r="M10" s="37">
+      <c r="M10" s="17">
         <v>5</v>
       </c>
-      <c r="N10" s="37">
+      <c r="N10" s="17">
         <v>3</v>
       </c>
-      <c r="O10" s="37">
+      <c r="O10" s="17">
         <v>0</v>
       </c>
-      <c r="P10" s="37">
+      <c r="P10" s="17">
         <v>0</v>
       </c>
-      <c r="Q10" s="37">
+      <c r="Q10" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="44">
+      <c r="D11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="53">
         <v>6</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="55">
+      <c r="G11" s="54"/>
+      <c r="H11" s="25">
         <v>6</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="17">
         <v>6</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="17">
         <v>6</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="17">
         <v>6</v>
       </c>
-      <c r="L11" s="46">
+      <c r="L11" s="22">
         <v>6</v>
       </c>
-      <c r="M11" s="37">
+      <c r="M11" s="17">
         <v>6</v>
       </c>
-      <c r="N11" s="37">
+      <c r="N11" s="17">
         <v>6</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="17">
         <v>3</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="17">
         <v>0</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="44">
+        <v>42</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="53">
         <v>5</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="55">
+      <c r="G12" s="54"/>
+      <c r="H12" s="25">
         <v>5</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="17">
         <v>5</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="17">
         <v>5</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="17">
         <v>5</v>
       </c>
-      <c r="L12" s="37">
+      <c r="L12" s="17">
         <v>5</v>
       </c>
-      <c r="M12" s="37">
+      <c r="M12" s="17">
         <v>5</v>
       </c>
-      <c r="N12" s="37">
+      <c r="N12" s="17">
         <v>5</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="17">
         <v>5</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="17">
         <v>3</v>
       </c>
-      <c r="Q12" s="37">
+      <c r="Q12" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="44">
+      <c r="D13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="53">
         <v>5</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="55">
+      <c r="G13" s="54"/>
+      <c r="H13" s="25">
         <v>5</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="17">
         <v>5</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="17">
         <v>5</v>
       </c>
-      <c r="K13" s="37">
+      <c r="K13" s="17">
         <v>5</v>
       </c>
-      <c r="L13" s="37">
+      <c r="L13" s="17">
         <v>5</v>
       </c>
-      <c r="M13" s="37">
+      <c r="M13" s="17">
         <v>5</v>
       </c>
-      <c r="N13" s="37">
+      <c r="N13" s="17">
         <v>5</v>
       </c>
-      <c r="O13" s="37">
+      <c r="O13" s="17">
         <v>5</v>
       </c>
-      <c r="P13" s="37">
+      <c r="P13" s="17">
         <v>3</v>
       </c>
-      <c r="Q13" s="37">
+      <c r="Q13" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F14" s="47">
+      <c r="F14" s="23">
         <f>SUM(F8:F13)</f>
         <v>35</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47">
+      <c r="G14" s="23"/>
+      <c r="H14" s="23">
         <f>SUM(H8:H13)</f>
         <v>35</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="23">
         <f>SUM(I8:I13)</f>
         <v>35</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="23">
         <f t="shared" ref="J14:Q14" si="0">SUM(J8:J13)</f>
         <v>31</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="23">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="L14" s="47">
+      <c r="L14" s="23">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="M14" s="47">
+      <c r="M14" s="23">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="N14" s="47">
+      <c r="N14" s="23">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="O14" s="47">
+      <c r="O14" s="23">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="P14" s="47">
+      <c r="P14" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="Q14" s="47">
+      <c r="Q14" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="56">
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="26">
         <v>35</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="23">
         <f>F14-($F$14/9)</f>
         <v>31.111111111111111</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="23">
         <f>I15-($F$14/9)</f>
         <v>27.222222222222221</v>
       </c>
-      <c r="K15" s="47">
+      <c r="K15" s="23">
         <f t="shared" ref="K15:Q15" si="1">J15-($F$14/9)</f>
         <v>23.333333333333332</v>
       </c>
-      <c r="L15" s="47">
+      <c r="L15" s="23">
         <f t="shared" si="1"/>
         <v>19.444444444444443</v>
       </c>
-      <c r="M15" s="47">
+      <c r="M15" s="23">
         <f t="shared" si="1"/>
         <v>15.555555555555554</v>
       </c>
-      <c r="N15" s="47">
+      <c r="N15" s="23">
         <f t="shared" si="1"/>
         <v>11.666666666666664</v>
       </c>
-      <c r="O15" s="47">
+      <c r="O15" s="23">
         <f t="shared" si="1"/>
         <v>7.777777777777775</v>
       </c>
-      <c r="P15" s="47">
+      <c r="P15" s="23">
         <f t="shared" si="1"/>
         <v>3.8888888888888862</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>